<commit_message>
docs: added work plan update(main file is in OneDrive)
</commit_message>
<xml_diff>
--- a/Gantt-Chart-Work-Plan.xlsx
+++ b/Gantt-Chart-Work-Plan.xlsx
@@ -1,15 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26330"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01113995-D04B-4402-A2CF-29D2C6781E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3784F6A0-4AC1-443A-9BDA-5CD7829641F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
-    <sheet name="About" sheetId="12" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Display_Week">ProjectSchedule!$E$4</definedName>
@@ -43,10 +42,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={0E61EB6B-9332-4750-A457-CFC809416494}</author>
+    <author>tc={6C08D0E6-C28E-4D2B-91EA-08E227A5197F}</author>
   </authors>
   <commentList>
-    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{0E61EB6B-9332-4750-A457-CFC809416494}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{6C08D0E6-C28E-4D2B-91EA-08E227A5197F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -59,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="60">
   <si>
     <t>Create a Project Schedule in this worksheet.
 Enter title of this project in cell B1. 
@@ -70,7 +69,7 @@
     <t>CSYM026 Assessment Project</t>
   </si>
   <si>
-    <t xml:space="preserve">NOTES: Please notify me if you have updates or tasks that we should list ⚠️.   </t>
+    <t xml:space="preserve">NOTE: Please notify me if you have updates or tasks that we should list ⚠️.   </t>
   </si>
   <si>
     <t>Enter Company Name in cell B2.</t>
@@ -79,7 +78,7 @@
     <t>GROUP 6</t>
   </si>
   <si>
-    <t>Purple = Not done, Green= Done</t>
+    <t>Purple = Not done, Green= Done, Blue = Project start</t>
   </si>
   <si>
     <t>Enter the name of the Project Lead in cell B3. Enter the Project Start date in cell E3. Pooject Start: label is in cell C3.</t>
@@ -94,7 +93,7 @@
 Display Week: label is in cell C4.</t>
   </si>
   <si>
-    <t>Team Members: Airat Yusuff, Gold Okpa, Alen Varghese</t>
+    <t>Team Members: Airat, Gold, Alen</t>
   </si>
   <si>
     <t>Display Week:</t>
@@ -215,19 +214,22 @@
     <t>Stage 1 Testing: write JUnit tests for the classes</t>
   </si>
   <si>
+    <t>Refactor and update tests</t>
+  </si>
+  <si>
     <t>Sample phase title block</t>
   </si>
   <si>
     <t>Stage 1 Group Report (Refer to Brief)</t>
   </si>
   <si>
-    <t>Section 1 &amp; 5</t>
+    <t>Section 1, 2 &amp; 5</t>
   </si>
   <si>
-    <t>Section 2 &amp; 3</t>
+    <t>Section 3 &amp; 4</t>
   </si>
   <si>
-    <t>Section 4 &amp; 6</t>
+    <t>Section 6</t>
   </si>
   <si>
     <t>Overall review/revision</t>
@@ -245,7 +247,7 @@
     <t>Stage 2 Planning</t>
   </si>
   <si>
-    <t>Task 1</t>
+    <t>Meeting to highlight tasks and sprints</t>
   </si>
   <si>
     <t>Task 2</t>
@@ -272,56 +274,6 @@
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
-  <si>
-    <t>SIMPLE GANTT CHART by Vertex42.com</t>
-  </si>
-  <si>
-    <t>https://www.vertex42.com/ExcelTemplates/simple-gantt-chart.html</t>
-  </si>
-  <si>
-    <t>About This Template</t>
-  </si>
-  <si>
-    <t>This template provides a simple way to create a Gantt chart to help visualise and track your project. Simply enter your tasks and start and end dates - no formulae required. The bars in the Gantt chart represent the duration of the task and are displayed using conditional formatting. Insert new tasks by inserting new rows.</t>
-  </si>
-  <si>
-    <t>Guide for Screen Readers</t>
-  </si>
-  <si>
-    <t>There are 2 worksheets in this workbook. 
-TimeSheet
-About
-The instructions for each worksheet are in the A column starting in cell A1 of each worksheet. They are written with hidden text. Each step guides you through the information in that row. Each subsequent step continues in cell A2, A3, and so on, unless otherwise explicitly directed. For example, instruction text might say "continue to cell A6" for the next step. 
-This hidden text will not print.
-To remove these instructions from the worksheet, simply delete column A.</t>
-  </si>
-  <si>
-    <t>Additional Help</t>
-  </si>
-  <si>
-    <t>Click on the link below to visit vertex42.com and learn more about how to use this template, such as how to calculate days and work days, create task dependencies, change the colours of the bars, add a scroll bar to make it easier to change the display week, extend the date range displayed in the chart, etc.</t>
-  </si>
-  <si>
-    <t>How to Use the Simple Gantt Chart</t>
-  </si>
-  <si>
-    <t>More Project Management Templates</t>
-  </si>
-  <si>
-    <t>Visit Vertex42.com to download other project management templates, including different types of project schedules, Gantt charts, tasks lists, etc.</t>
-  </si>
-  <si>
-    <t>Project Management Templates</t>
-  </si>
-  <si>
-    <t>About Vertex42</t>
-  </si>
-  <si>
-    <t>Vertex42.com provides over 300 professionally designed spreadsheet templates for business, home, and education - most of which are free to download. Their collection includes a variety of calendars, planners, and schedules as well as personal finance spreadsheets for budgeting, debt reduction, and loan amortisation.</t>
-  </si>
-  <si>
-    <t>Businesses will find invoices, time sheets, inventory trackers, financial statements, and project planning templates. Teachers and students will find resources such as class schedules, grade books, and attendance sheets. Organise your family life with meal planners, checklists, and exercise logs. Each template is thoroughly researched, refined, and improved over time through feedback from thousands of users.</t>
-  </si>
 </sst>
 </file>
 
@@ -337,7 +289,7 @@
     <numFmt numFmtId="168" formatCode="d"/>
     <numFmt numFmtId="169" formatCode="d\ mmm\ yyyy"/>
   </numFmts>
-  <fonts count="39">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -453,49 +405,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1" tint="0.34998626667073579"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1" tint="0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF1D2129"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -609,6 +518,7 @@
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1085,7 +995,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="3" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1107,49 +1017,49 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyFill="0">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="19" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="20" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1247,39 +1157,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1335,11 +1217,8 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1396,6 +1275,10 @@
     <xf numFmtId="168" fontId="11" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="45" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="169" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1404,10 +1287,6 @@
     </xf>
     <xf numFmtId="169" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="45" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
@@ -1475,7 +1354,67 @@
     <cellStyle name="Warning Text" xfId="26" builtinId="11" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF548235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1602,15 +1541,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="11"/>
-      <tableStyleElement type="headerRow" dxfId="10"/>
-      <tableStyleElement type="totalRow" dxfId="9"/>
-      <tableStyleElement type="firstColumn" dxfId="8"/>
-      <tableStyleElement type="lastColumn" dxfId="7"/>
-      <tableStyleElement type="firstRowStripe" dxfId="6"/>
-      <tableStyleElement type="secondRowStripe" dxfId="5"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="4"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="3"/>
+      <tableStyleElement type="wholeTable" dxfId="17"/>
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="firstColumn" dxfId="14"/>
+      <tableStyleElement type="lastColumn" dxfId="13"/>
+      <tableStyleElement type="firstRowStripe" dxfId="12"/>
+      <tableStyleElement type="secondRowStripe" dxfId="11"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="9"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1701,68 +1640,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1905000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>523875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Vertex42 logo">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="190500" y="95250"/>
-          <a:ext cx="1905000" cy="428625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Yusuff Airat" id="{17D4AA1B-E2E8-4D31-ACEE-B773D3B1AF6B}" userId="S::airat.yusuff22@my.northampton.ac.uk::05eb4885-b139-4b8e-b0ba-335e8a3ea425" providerId="AD"/>
-</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2028,7 +1905,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D11" dT="2023-03-29T18:28:15.78" personId="{17D4AA1B-E2E8-4D31-ACEE-B773D3B1AF6B}" id="{0E61EB6B-9332-4750-A457-CFC809416494}">
+  <threadedComment ref="C1" dT="2023-03-29T18:45:20.35" personId="{00000000-0000-0000-0000-000000000000}" id="{6C08D0E6-C28E-4D2B-91EA-08E227A5197F}">
     <text>@alen.varghese22@my.northampton.ac.uk @gold.okpa22@my.northampton.ac.uk see the new work plan</text>
   </threadedComment>
 </ThreadedComments>
@@ -2039,32 +1916,31 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL41"/>
+  <dimension ref="A1:BZ42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB28" sqref="AB28"/>
+      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="45" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="35" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" style="5" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" customWidth="1"/>
     <col min="7" max="7" width="2.7109375" customWidth="1"/>
     <col min="8" max="8" width="6.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="64" width="2.42578125" customWidth="1"/>
-    <col min="69" max="70" width="10.28515625"/>
+    <col min="9" max="78" width="2.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="30" customHeight="1">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:78" ht="24.75" customHeight="1">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1"/>
@@ -2072,370 +1948,446 @@
       <c r="E1" s="4"/>
       <c r="F1" s="34"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="91" t="s">
+      <c r="I1" s="57"/>
+      <c r="J1" s="77" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1">
-      <c r="A2" s="45" t="s">
+    <row r="2" spans="1:78" ht="23.25" customHeight="1">
+      <c r="A2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="68"/>
+      <c r="I2" s="58"/>
       <c r="M2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:64" ht="30" customHeight="1">
-      <c r="A3" s="45" t="s">
+    <row r="3" spans="1:78" ht="24" customHeight="1">
+      <c r="A3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="93" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="94"/>
-      <c r="E3" s="95">
-        <f ca="1">TODAY() - 8</f>
+      <c r="D3" s="83"/>
+      <c r="E3" s="84">
+        <f>DATE(2023,3,21)</f>
         <v>45006</v>
       </c>
-      <c r="F3" s="95"/>
+      <c r="F3" s="84"/>
     </row>
-    <row r="4" spans="1:64" ht="30" customHeight="1">
-      <c r="A4" s="46" t="s">
+    <row r="4" spans="1:78" ht="24" customHeight="1">
+      <c r="A4" s="36" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="93" t="s">
+      <c r="C4" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="94"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="88">
-        <f ca="1">I5</f>
+      <c r="I4" s="79">
+        <f>I5</f>
         <v>45005</v>
       </c>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="88">
-        <f ca="1">P5</f>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="79">
+        <f>P5</f>
         <v>45012</v>
       </c>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="89"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="88">
-        <f ca="1">W5</f>
+      <c r="Q4" s="80"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="80"/>
+      <c r="T4" s="80"/>
+      <c r="U4" s="80"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="79">
+        <f>W5</f>
         <v>45019</v>
       </c>
-      <c r="X4" s="89"/>
-      <c r="Y4" s="89"/>
-      <c r="Z4" s="89"/>
-      <c r="AA4" s="89"/>
-      <c r="AB4" s="89"/>
-      <c r="AC4" s="90"/>
-      <c r="AD4" s="88">
-        <f ca="1">AD5</f>
+      <c r="X4" s="80"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="80"/>
+      <c r="AA4" s="80"/>
+      <c r="AB4" s="80"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="79">
+        <f>AD5</f>
         <v>45026</v>
       </c>
-      <c r="AE4" s="89"/>
-      <c r="AF4" s="89"/>
-      <c r="AG4" s="89"/>
-      <c r="AH4" s="89"/>
-      <c r="AI4" s="89"/>
-      <c r="AJ4" s="90"/>
-      <c r="AK4" s="88">
-        <f ca="1">AK5</f>
+      <c r="AE4" s="80"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="80"/>
+      <c r="AH4" s="80"/>
+      <c r="AI4" s="80"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="79">
+        <f>AK5</f>
         <v>45033</v>
       </c>
-      <c r="AL4" s="89"/>
-      <c r="AM4" s="89"/>
-      <c r="AN4" s="89"/>
-      <c r="AO4" s="89"/>
-      <c r="AP4" s="89"/>
-      <c r="AQ4" s="90"/>
-      <c r="AR4" s="88">
-        <f ca="1">AR5</f>
+      <c r="AL4" s="80"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="80"/>
+      <c r="AO4" s="80"/>
+      <c r="AP4" s="80"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="79">
+        <f>AR5</f>
         <v>45040</v>
       </c>
-      <c r="AS4" s="89"/>
-      <c r="AT4" s="89"/>
-      <c r="AU4" s="89"/>
-      <c r="AV4" s="89"/>
-      <c r="AW4" s="89"/>
-      <c r="AX4" s="90"/>
-      <c r="AY4" s="88">
-        <f ca="1">AY5</f>
+      <c r="AS4" s="80"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="80"/>
+      <c r="AV4" s="80"/>
+      <c r="AW4" s="80"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="79">
+        <f>AY5</f>
         <v>45047</v>
       </c>
-      <c r="AZ4" s="89"/>
-      <c r="BA4" s="89"/>
-      <c r="BB4" s="89"/>
-      <c r="BC4" s="89"/>
-      <c r="BD4" s="89"/>
-      <c r="BE4" s="90"/>
-      <c r="BF4" s="88">
-        <f ca="1">BF5</f>
+      <c r="AZ4" s="80"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="80"/>
+      <c r="BC4" s="80"/>
+      <c r="BD4" s="80"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="79">
+        <f>BF5</f>
         <v>45054</v>
       </c>
-      <c r="BG4" s="89"/>
-      <c r="BH4" s="89"/>
-      <c r="BI4" s="89"/>
-      <c r="BJ4" s="89"/>
-      <c r="BK4" s="89"/>
-      <c r="BL4" s="90"/>
+      <c r="BG4" s="80"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="80"/>
+      <c r="BJ4" s="80"/>
+      <c r="BK4" s="80"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="79">
+        <f>BM5</f>
+        <v>45061</v>
+      </c>
+      <c r="BN4" s="80"/>
+      <c r="BO4" s="80"/>
+      <c r="BP4" s="80"/>
+      <c r="BQ4" s="80"/>
+      <c r="BR4" s="80"/>
+      <c r="BS4" s="81"/>
+      <c r="BT4" s="79">
+        <f>BT5</f>
+        <v>45068</v>
+      </c>
+      <c r="BU4" s="80"/>
+      <c r="BV4" s="80"/>
+      <c r="BW4" s="80"/>
+      <c r="BX4" s="80"/>
+      <c r="BY4" s="80"/>
+      <c r="BZ4" s="81"/>
     </row>
-    <row r="5" spans="1:64" ht="15" customHeight="1">
-      <c r="A5" s="46" t="s">
+    <row r="5" spans="1:78" ht="15" customHeight="1">
+      <c r="A5" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="I5" s="85">
-        <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="I5" s="74">
+        <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>45005</v>
       </c>
-      <c r="J5" s="86">
-        <f ca="1">I5+1</f>
+      <c r="J5" s="75">
+        <f>I5+1</f>
         <v>45006</v>
       </c>
-      <c r="K5" s="86">
-        <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
+      <c r="K5" s="75">
+        <f t="shared" ref="K5:AX5" si="0">J5+1</f>
         <v>45007</v>
       </c>
-      <c r="L5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="L5" s="75">
+        <f t="shared" si="0"/>
         <v>45008</v>
       </c>
-      <c r="M5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="M5" s="75">
+        <f t="shared" si="0"/>
         <v>45009</v>
       </c>
-      <c r="N5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="N5" s="75">
+        <f t="shared" si="0"/>
         <v>45010</v>
       </c>
-      <c r="O5" s="87">
-        <f t="shared" ca="1" si="0"/>
+      <c r="O5" s="76">
+        <f t="shared" si="0"/>
         <v>45011</v>
       </c>
-      <c r="P5" s="85">
-        <f ca="1">O5+1</f>
+      <c r="P5" s="74">
+        <f>O5+1</f>
         <v>45012</v>
       </c>
-      <c r="Q5" s="86">
-        <f ca="1">P5+1</f>
+      <c r="Q5" s="75">
+        <f>P5+1</f>
         <v>45013</v>
       </c>
-      <c r="R5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="R5" s="75">
+        <f t="shared" si="0"/>
         <v>45014</v>
       </c>
-      <c r="S5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="S5" s="75">
+        <f t="shared" si="0"/>
         <v>45015</v>
       </c>
-      <c r="T5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="T5" s="75">
+        <f t="shared" si="0"/>
         <v>45016</v>
       </c>
-      <c r="U5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="U5" s="75">
+        <f t="shared" si="0"/>
         <v>45017</v>
       </c>
-      <c r="V5" s="87">
-        <f t="shared" ca="1" si="0"/>
+      <c r="V5" s="76">
+        <f t="shared" si="0"/>
         <v>45018</v>
       </c>
-      <c r="W5" s="85">
-        <f ca="1">V5+1</f>
+      <c r="W5" s="74">
+        <f>V5+1</f>
         <v>45019</v>
       </c>
-      <c r="X5" s="86">
-        <f ca="1">W5+1</f>
+      <c r="X5" s="75">
+        <f>W5+1</f>
         <v>45020</v>
       </c>
-      <c r="Y5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="Y5" s="75">
+        <f t="shared" si="0"/>
         <v>45021</v>
       </c>
-      <c r="Z5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="Z5" s="75">
+        <f t="shared" si="0"/>
         <v>45022</v>
       </c>
-      <c r="AA5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AA5" s="75">
+        <f t="shared" si="0"/>
         <v>45023</v>
       </c>
-      <c r="AB5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AB5" s="75">
+        <f t="shared" si="0"/>
         <v>45024</v>
       </c>
-      <c r="AC5" s="87">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AC5" s="76">
+        <f t="shared" si="0"/>
         <v>45025</v>
       </c>
-      <c r="AD5" s="85">
-        <f ca="1">AC5+1</f>
+      <c r="AD5" s="74">
+        <f>AC5+1</f>
         <v>45026</v>
       </c>
-      <c r="AE5" s="86">
-        <f ca="1">AD5+1</f>
+      <c r="AE5" s="75">
+        <f>AD5+1</f>
         <v>45027</v>
       </c>
-      <c r="AF5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AF5" s="75">
+        <f t="shared" si="0"/>
         <v>45028</v>
       </c>
-      <c r="AG5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AG5" s="75">
+        <f t="shared" si="0"/>
         <v>45029</v>
       </c>
-      <c r="AH5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AH5" s="75">
+        <f t="shared" si="0"/>
         <v>45030</v>
       </c>
-      <c r="AI5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AI5" s="75">
+        <f t="shared" si="0"/>
         <v>45031</v>
       </c>
-      <c r="AJ5" s="87">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AJ5" s="76">
+        <f t="shared" si="0"/>
         <v>45032</v>
       </c>
-      <c r="AK5" s="85">
-        <f ca="1">AJ5+1</f>
+      <c r="AK5" s="74">
+        <f>AJ5+1</f>
         <v>45033</v>
       </c>
-      <c r="AL5" s="86">
-        <f ca="1">AK5+1</f>
+      <c r="AL5" s="75">
+        <f>AK5+1</f>
         <v>45034</v>
       </c>
-      <c r="AM5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AM5" s="75">
+        <f t="shared" si="0"/>
         <v>45035</v>
       </c>
-      <c r="AN5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AN5" s="75">
+        <f t="shared" si="0"/>
         <v>45036</v>
       </c>
-      <c r="AO5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AO5" s="75">
+        <f t="shared" si="0"/>
         <v>45037</v>
       </c>
-      <c r="AP5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AP5" s="75">
+        <f t="shared" si="0"/>
         <v>45038</v>
       </c>
-      <c r="AQ5" s="87">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AQ5" s="76">
+        <f t="shared" si="0"/>
         <v>45039</v>
       </c>
-      <c r="AR5" s="85">
-        <f ca="1">AQ5+1</f>
+      <c r="AR5" s="74">
+        <f>AQ5+1</f>
         <v>45040</v>
       </c>
-      <c r="AS5" s="86">
-        <f ca="1">AR5+1</f>
+      <c r="AS5" s="75">
+        <f>AR5+1</f>
         <v>45041</v>
       </c>
-      <c r="AT5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AT5" s="75">
+        <f t="shared" si="0"/>
         <v>45042</v>
       </c>
-      <c r="AU5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AU5" s="75">
+        <f t="shared" si="0"/>
         <v>45043</v>
       </c>
-      <c r="AV5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AV5" s="75">
+        <f t="shared" si="0"/>
         <v>45044</v>
       </c>
-      <c r="AW5" s="86">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AW5" s="75">
+        <f t="shared" si="0"/>
         <v>45045</v>
       </c>
-      <c r="AX5" s="87">
-        <f t="shared" ca="1" si="0"/>
+      <c r="AX5" s="76">
+        <f t="shared" si="0"/>
         <v>45046</v>
       </c>
-      <c r="AY5" s="85">
-        <f ca="1">AX5+1</f>
+      <c r="AY5" s="74">
+        <f>AX5+1</f>
         <v>45047</v>
       </c>
-      <c r="AZ5" s="86">
-        <f ca="1">AY5+1</f>
+      <c r="AZ5" s="75">
+        <f>AY5+1</f>
         <v>45048</v>
       </c>
-      <c r="BA5" s="86">
-        <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
+      <c r="BA5" s="75">
+        <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
         <v>45049</v>
       </c>
-      <c r="BB5" s="86">
-        <f t="shared" ca="1" si="1"/>
+      <c r="BB5" s="75">
+        <f t="shared" si="1"/>
         <v>45050</v>
       </c>
-      <c r="BC5" s="86">
-        <f t="shared" ca="1" si="1"/>
+      <c r="BC5" s="75">
+        <f t="shared" si="1"/>
         <v>45051</v>
       </c>
-      <c r="BD5" s="86">
-        <f t="shared" ca="1" si="1"/>
+      <c r="BD5" s="75">
+        <f t="shared" si="1"/>
         <v>45052</v>
       </c>
-      <c r="BE5" s="87">
-        <f t="shared" ca="1" si="1"/>
+      <c r="BE5" s="76">
+        <f t="shared" si="1"/>
         <v>45053</v>
       </c>
-      <c r="BF5" s="85">
-        <f ca="1">BE5+1</f>
+      <c r="BF5" s="74">
+        <f>BE5+1</f>
         <v>45054</v>
       </c>
-      <c r="BG5" s="86">
-        <f ca="1">BF5+1</f>
+      <c r="BG5" s="75">
+        <f>BF5+1</f>
         <v>45055</v>
       </c>
-      <c r="BH5" s="86">
-        <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
+      <c r="BH5" s="75">
+        <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
         <v>45056</v>
       </c>
-      <c r="BI5" s="86">
-        <f t="shared" ca="1" si="2"/>
+      <c r="BI5" s="75">
+        <f t="shared" si="2"/>
         <v>45057</v>
       </c>
-      <c r="BJ5" s="86">
-        <f t="shared" ca="1" si="2"/>
+      <c r="BJ5" s="75">
+        <f t="shared" si="2"/>
         <v>45058</v>
       </c>
-      <c r="BK5" s="86">
-        <f t="shared" ca="1" si="2"/>
+      <c r="BK5" s="75">
+        <f t="shared" si="2"/>
         <v>45059</v>
       </c>
-      <c r="BL5" s="87">
-        <f t="shared" ca="1" si="2"/>
+      <c r="BL5" s="76">
+        <f t="shared" si="2"/>
         <v>45060</v>
       </c>
+      <c r="BM5" s="74">
+        <f>BL5+1</f>
+        <v>45061</v>
+      </c>
+      <c r="BN5" s="75">
+        <f>BM5+1</f>
+        <v>45062</v>
+      </c>
+      <c r="BO5" s="75">
+        <f t="shared" ref="BO5" si="3">BN5+1</f>
+        <v>45063</v>
+      </c>
+      <c r="BP5" s="75">
+        <f t="shared" ref="BP5" si="4">BO5+1</f>
+        <v>45064</v>
+      </c>
+      <c r="BQ5" s="75">
+        <f t="shared" ref="BQ5" si="5">BP5+1</f>
+        <v>45065</v>
+      </c>
+      <c r="BR5" s="75">
+        <f t="shared" ref="BR5" si="6">BQ5+1</f>
+        <v>45066</v>
+      </c>
+      <c r="BS5" s="76">
+        <f t="shared" ref="BS5" si="7">BR5+1</f>
+        <v>45067</v>
+      </c>
+      <c r="BT5" s="74">
+        <f>BS5+1</f>
+        <v>45068</v>
+      </c>
+      <c r="BU5" s="75">
+        <f>BT5+1</f>
+        <v>45069</v>
+      </c>
+      <c r="BV5" s="75">
+        <f t="shared" ref="BV5" si="8">BU5+1</f>
+        <v>45070</v>
+      </c>
+      <c r="BW5" s="75">
+        <f t="shared" ref="BW5" si="9">BV5+1</f>
+        <v>45071</v>
+      </c>
+      <c r="BX5" s="75">
+        <f t="shared" ref="BX5" si="10">BW5+1</f>
+        <v>45072</v>
+      </c>
+      <c r="BY5" s="75">
+        <f t="shared" ref="BY5" si="11">BX5+1</f>
+        <v>45073</v>
+      </c>
+      <c r="BZ5" s="76">
+        <f t="shared" ref="BZ5" si="12">BY5+1</f>
+        <v>45074</v>
+      </c>
     </row>
-    <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1">
-      <c r="A6" s="46" t="s">
+    <row r="6" spans="1:78" ht="30" customHeight="1">
+      <c r="A6" s="36" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -2458,235 +2410,291 @@
         <v>18</v>
       </c>
       <c r="I6" s="10" t="str">
-        <f t="shared" ref="I6" ca="1" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
+        <f t="shared" ref="I6" si="13">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
       </c>
       <c r="J6" s="10" t="str">
-        <f t="shared" ref="J6:AR6" ca="1" si="4">LEFT(TEXT(J5,"ddd"),1)</f>
+        <f t="shared" ref="J6:AR6" si="14">LEFT(TEXT(J5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="K6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>W</v>
       </c>
       <c r="L6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>T</v>
       </c>
       <c r="M6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>F</v>
       </c>
       <c r="N6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>S</v>
       </c>
       <c r="O6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>S</v>
       </c>
       <c r="P6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>M</v>
       </c>
       <c r="Q6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>T</v>
       </c>
       <c r="R6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>W</v>
       </c>
       <c r="S6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>T</v>
       </c>
       <c r="T6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>F</v>
       </c>
       <c r="U6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>S</v>
       </c>
       <c r="V6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>S</v>
       </c>
       <c r="W6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>M</v>
       </c>
       <c r="X6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>T</v>
       </c>
       <c r="Y6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>W</v>
       </c>
       <c r="Z6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>T</v>
       </c>
       <c r="AA6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>F</v>
       </c>
       <c r="AB6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>S</v>
       </c>
       <c r="AC6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>S</v>
       </c>
       <c r="AD6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>M</v>
       </c>
       <c r="AE6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>T</v>
       </c>
       <c r="AF6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>W</v>
       </c>
       <c r="AG6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>T</v>
       </c>
       <c r="AH6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>F</v>
       </c>
       <c r="AI6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>S</v>
       </c>
       <c r="AJ6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>S</v>
       </c>
       <c r="AK6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>M</v>
       </c>
       <c r="AL6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>T</v>
       </c>
       <c r="AM6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>W</v>
       </c>
       <c r="AN6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>T</v>
       </c>
       <c r="AO6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>F</v>
       </c>
       <c r="AP6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>S</v>
       </c>
       <c r="AQ6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>S</v>
       </c>
       <c r="AR6" s="10" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="14"/>
         <v>M</v>
       </c>
       <c r="AS6" s="10" t="str">
-        <f t="shared" ref="AS6:BL6" ca="1" si="5">LEFT(TEXT(AS5,"ddd"),1)</f>
+        <f t="shared" ref="AS6:BL6" si="15">LEFT(TEXT(AS5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="AT6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>W</v>
       </c>
       <c r="AU6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>T</v>
       </c>
       <c r="AV6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>F</v>
       </c>
       <c r="AW6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>S</v>
       </c>
       <c r="AX6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>S</v>
       </c>
       <c r="AY6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>M</v>
       </c>
       <c r="AZ6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>T</v>
       </c>
       <c r="BA6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>W</v>
       </c>
       <c r="BB6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>T</v>
       </c>
       <c r="BC6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>F</v>
       </c>
       <c r="BD6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>S</v>
       </c>
       <c r="BE6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>S</v>
       </c>
       <c r="BF6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>M</v>
       </c>
       <c r="BG6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>T</v>
       </c>
       <c r="BH6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>W</v>
       </c>
       <c r="BI6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>T</v>
       </c>
       <c r="BJ6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>F</v>
       </c>
       <c r="BK6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>S</v>
       </c>
       <c r="BL6" s="10" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="15"/>
         <v>S</v>
       </c>
+      <c r="BM6" s="10" t="str">
+        <f t="shared" ref="BM6:BZ6" si="16">LEFT(TEXT(BM5,"ddd"),1)</f>
+        <v>M</v>
+      </c>
+      <c r="BN6" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>T</v>
+      </c>
+      <c r="BO6" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>W</v>
+      </c>
+      <c r="BP6" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>T</v>
+      </c>
+      <c r="BQ6" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>F</v>
+      </c>
+      <c r="BR6" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>S</v>
+      </c>
+      <c r="BS6" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>S</v>
+      </c>
+      <c r="BT6" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>M</v>
+      </c>
+      <c r="BU6" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>T</v>
+      </c>
+      <c r="BV6" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>W</v>
+      </c>
+      <c r="BW6" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>T</v>
+      </c>
+      <c r="BX6" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>F</v>
+      </c>
+      <c r="BY6" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>S</v>
+      </c>
+      <c r="BZ6" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>S</v>
+      </c>
     </row>
-    <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1">
-      <c r="A7" s="45" t="s">
+    <row r="7" spans="1:78" ht="30" hidden="1" customHeight="1">
+      <c r="A7" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="48"/>
+      <c r="C7" s="38"/>
       <c r="E7"/>
       <c r="H7" t="str">
         <f ca="1">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
@@ -2748,21 +2756,35 @@
       <c r="BJ7" s="31"/>
       <c r="BK7" s="31"/>
       <c r="BL7" s="31"/>
+      <c r="BM7" s="31"/>
+      <c r="BN7" s="31"/>
+      <c r="BO7" s="31"/>
+      <c r="BP7" s="31"/>
+      <c r="BQ7" s="31"/>
+      <c r="BR7" s="31"/>
+      <c r="BS7" s="31"/>
+      <c r="BT7" s="31"/>
+      <c r="BU7" s="31"/>
+      <c r="BV7" s="31"/>
+      <c r="BW7" s="31"/>
+      <c r="BX7" s="31"/>
+      <c r="BY7" s="31"/>
+      <c r="BZ7" s="31"/>
     </row>
-    <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A8" s="46" t="s">
+    <row r="8" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A8" s="36" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="52"/>
+      <c r="C8" s="42"/>
       <c r="D8" s="16"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="71"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="str">
-        <f t="shared" ref="H8:H38" ca="1" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H39" ca="1" si="17">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="31"/>
@@ -2821,36 +2843,50 @@
       <c r="BJ8" s="31"/>
       <c r="BK8" s="31"/>
       <c r="BL8" s="31"/>
+      <c r="BM8" s="31"/>
+      <c r="BN8" s="31"/>
+      <c r="BO8" s="31"/>
+      <c r="BP8" s="31"/>
+      <c r="BQ8" s="31"/>
+      <c r="BR8" s="31"/>
+      <c r="BS8" s="31"/>
+      <c r="BT8" s="31"/>
+      <c r="BU8" s="31"/>
+      <c r="BV8" s="31"/>
+      <c r="BW8" s="31"/>
+      <c r="BX8" s="31"/>
+      <c r="BY8" s="31"/>
+      <c r="BZ8" s="31"/>
     </row>
-    <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A9" s="46" t="s">
+    <row r="9" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A9" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="43" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="17">
         <v>1</v>
       </c>
-      <c r="E9" s="72">
-        <f ca="1">Project_Start+1</f>
+      <c r="E9" s="61">
+        <f>Project_Start+1</f>
         <v>45007</v>
       </c>
-      <c r="F9" s="72">
-        <f ca="1">E9</f>
+      <c r="F9" s="61">
+        <f>E9</f>
         <v>45007</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="17"/>
         <v>1</v>
       </c>
       <c r="I9" s="31"/>
       <c r="J9" s="31"/>
-      <c r="K9" s="92"/>
+      <c r="K9" s="78"/>
       <c r="L9" s="31"/>
       <c r="M9" s="31"/>
       <c r="N9" s="31"/>
@@ -2904,32 +2940,46 @@
       <c r="BJ9" s="31"/>
       <c r="BK9" s="31"/>
       <c r="BL9" s="31"/>
+      <c r="BM9" s="31"/>
+      <c r="BN9" s="31"/>
+      <c r="BO9" s="31"/>
+      <c r="BP9" s="31"/>
+      <c r="BQ9" s="31"/>
+      <c r="BR9" s="31"/>
+      <c r="BS9" s="31"/>
+      <c r="BT9" s="31"/>
+      <c r="BU9" s="31"/>
+      <c r="BV9" s="31"/>
+      <c r="BW9" s="31"/>
+      <c r="BX9" s="31"/>
+      <c r="BY9" s="31"/>
+      <c r="BZ9" s="31"/>
     </row>
-    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="46" t="s">
+    <row r="10" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A10" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="43" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="17">
         <v>0.5</v>
       </c>
-      <c r="E10" s="72">
-        <f ca="1">F9</f>
+      <c r="E10" s="61">
+        <f>F9</f>
         <v>45007</v>
       </c>
-      <c r="F10" s="72">
-        <f ca="1">E10+7</f>
-        <v>45014</v>
+      <c r="F10" s="61">
+        <f>E10+21</f>
+        <v>45028</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>8</v>
+        <f t="shared" ca="1" si="17"/>
+        <v>22</v>
       </c>
       <c r="I10" s="31"/>
       <c r="J10" s="31"/>
@@ -2987,25 +3037,39 @@
       <c r="BJ10" s="31"/>
       <c r="BK10" s="31"/>
       <c r="BL10" s="31"/>
+      <c r="BM10" s="31"/>
+      <c r="BN10" s="31"/>
+      <c r="BO10" s="31"/>
+      <c r="BP10" s="31"/>
+      <c r="BQ10" s="31"/>
+      <c r="BR10" s="31"/>
+      <c r="BS10" s="31"/>
+      <c r="BT10" s="31"/>
+      <c r="BU10" s="31"/>
+      <c r="BV10" s="31"/>
+      <c r="BW10" s="31"/>
+      <c r="BX10" s="31"/>
+      <c r="BY10" s="31"/>
+      <c r="BZ10" s="31"/>
     </row>
-    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="46"/>
-      <c r="B11" s="61" t="s">
+    <row r="11" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A11" s="36"/>
+      <c r="B11" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="43" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="17">
-        <v>0.9</v>
-      </c>
-      <c r="E11" s="72">
-        <f ca="1">E9</f>
+        <v>1</v>
+      </c>
+      <c r="E11" s="61">
+        <f>E9</f>
         <v>45007</v>
       </c>
-      <c r="F11" s="72">
-        <f ca="1">E11+1</f>
-        <v>45008</v>
+      <c r="F11" s="61">
+        <f>E11+2</f>
+        <v>45009</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -3065,29 +3129,43 @@
       <c r="BJ11" s="31"/>
       <c r="BK11" s="31"/>
       <c r="BL11" s="31"/>
+      <c r="BM11" s="31"/>
+      <c r="BN11" s="31"/>
+      <c r="BO11" s="31"/>
+      <c r="BP11" s="31"/>
+      <c r="BQ11" s="31"/>
+      <c r="BR11" s="31"/>
+      <c r="BS11" s="31"/>
+      <c r="BT11" s="31"/>
+      <c r="BU11" s="31"/>
+      <c r="BV11" s="31"/>
+      <c r="BW11" s="31"/>
+      <c r="BX11" s="31"/>
+      <c r="BY11" s="31"/>
+      <c r="BZ11" s="31"/>
     </row>
-    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A12" s="45"/>
-      <c r="B12" s="61" t="s">
+    <row r="12" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A12" s="35"/>
+      <c r="B12" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="43" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="17">
         <v>1</v>
       </c>
-      <c r="E12" s="72">
-        <f ca="1">E9</f>
+      <c r="E12" s="61">
+        <f>E9</f>
         <v>45007</v>
       </c>
-      <c r="F12" s="72">
-        <f ca="1">E12</f>
+      <c r="F12" s="61">
+        <f>E12</f>
         <v>45007</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="17"/>
         <v>1</v>
       </c>
       <c r="I12" s="31"/>
@@ -3146,24 +3224,38 @@
       <c r="BJ12" s="31"/>
       <c r="BK12" s="31"/>
       <c r="BL12" s="31"/>
+      <c r="BM12" s="31"/>
+      <c r="BN12" s="31"/>
+      <c r="BO12" s="31"/>
+      <c r="BP12" s="31"/>
+      <c r="BQ12" s="31"/>
+      <c r="BR12" s="31"/>
+      <c r="BS12" s="31"/>
+      <c r="BT12" s="31"/>
+      <c r="BU12" s="31"/>
+      <c r="BV12" s="31"/>
+      <c r="BW12" s="31"/>
+      <c r="BX12" s="31"/>
+      <c r="BY12" s="31"/>
+      <c r="BZ12" s="31"/>
     </row>
-    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A13" s="45"/>
-      <c r="B13" s="61" t="s">
+    <row r="13" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A13" s="35"/>
+      <c r="B13" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="53" t="s">
+      <c r="C13" s="43" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="17">
         <v>1</v>
       </c>
-      <c r="E13" s="72">
-        <f ca="1">E9</f>
+      <c r="E13" s="61">
+        <f>E9</f>
         <v>45007</v>
       </c>
-      <c r="F13" s="72">
-        <f ca="1">F17</f>
+      <c r="F13" s="61">
+        <f>F17</f>
         <v>45011</v>
       </c>
       <c r="G13" s="14"/>
@@ -3224,21 +3316,35 @@
       <c r="BJ13" s="31"/>
       <c r="BK13" s="31"/>
       <c r="BL13" s="31"/>
+      <c r="BM13" s="31"/>
+      <c r="BN13" s="31"/>
+      <c r="BO13" s="31"/>
+      <c r="BP13" s="31"/>
+      <c r="BQ13" s="31"/>
+      <c r="BR13" s="31"/>
+      <c r="BS13" s="31"/>
+      <c r="BT13" s="31"/>
+      <c r="BU13" s="31"/>
+      <c r="BV13" s="31"/>
+      <c r="BW13" s="31"/>
+      <c r="BX13" s="31"/>
+      <c r="BY13" s="31"/>
+      <c r="BZ13" s="31"/>
     </row>
-    <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A14" s="46" t="s">
+    <row r="14" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A14" s="36" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="52"/>
+      <c r="C14" s="42"/>
       <c r="D14" s="16"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="71"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="60"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="I14" s="31"/>
@@ -3297,24 +3403,38 @@
       <c r="BJ14" s="31"/>
       <c r="BK14" s="31"/>
       <c r="BL14" s="31"/>
+      <c r="BM14" s="31"/>
+      <c r="BN14" s="31"/>
+      <c r="BO14" s="31"/>
+      <c r="BP14" s="31"/>
+      <c r="BQ14" s="31"/>
+      <c r="BR14" s="31"/>
+      <c r="BS14" s="31"/>
+      <c r="BT14" s="31"/>
+      <c r="BU14" s="31"/>
+      <c r="BV14" s="31"/>
+      <c r="BW14" s="31"/>
+      <c r="BX14" s="31"/>
+      <c r="BY14" s="31"/>
+      <c r="BZ14" s="31"/>
     </row>
-    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A15" s="45"/>
-      <c r="B15" s="61" t="s">
+    <row r="15" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A15" s="35"/>
+      <c r="B15" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="43" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="20">
         <v>1</v>
       </c>
-      <c r="E15" s="72">
-        <f ca="1">F9+3</f>
+      <c r="E15" s="61">
+        <f>F9+3</f>
         <v>45010</v>
       </c>
-      <c r="F15" s="72">
-        <f ca="1">E15</f>
+      <c r="F15" s="61">
+        <f>E15</f>
         <v>45010</v>
       </c>
       <c r="G15" s="14"/>
@@ -3375,29 +3495,43 @@
       <c r="BJ15" s="31"/>
       <c r="BK15" s="31"/>
       <c r="BL15" s="31"/>
+      <c r="BM15" s="31"/>
+      <c r="BN15" s="31"/>
+      <c r="BO15" s="31"/>
+      <c r="BP15" s="31"/>
+      <c r="BQ15" s="31"/>
+      <c r="BR15" s="31"/>
+      <c r="BS15" s="31"/>
+      <c r="BT15" s="31"/>
+      <c r="BU15" s="31"/>
+      <c r="BV15" s="31"/>
+      <c r="BW15" s="31"/>
+      <c r="BX15" s="31"/>
+      <c r="BY15" s="31"/>
+      <c r="BZ15" s="31"/>
     </row>
-    <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A16" s="45"/>
-      <c r="B16" s="61" t="s">
+    <row r="16" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A16" s="35"/>
+      <c r="B16" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="43" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="20">
         <v>1</v>
       </c>
-      <c r="E16" s="72">
-        <f ca="1">E15</f>
+      <c r="E16" s="61">
+        <f>E15</f>
         <v>45010</v>
       </c>
-      <c r="F16" s="72">
-        <f ca="1">E16+1</f>
+      <c r="F16" s="61">
+        <f>E16+1</f>
         <v>45011</v>
       </c>
       <c r="G16" s="14"/>
       <c r="H16" s="14">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="17"/>
         <v>2</v>
       </c>
       <c r="I16" s="31"/>
@@ -3456,24 +3590,38 @@
       <c r="BJ16" s="31"/>
       <c r="BK16" s="31"/>
       <c r="BL16" s="31"/>
+      <c r="BM16" s="31"/>
+      <c r="BN16" s="31"/>
+      <c r="BO16" s="31"/>
+      <c r="BP16" s="31"/>
+      <c r="BQ16" s="31"/>
+      <c r="BR16" s="31"/>
+      <c r="BS16" s="31"/>
+      <c r="BT16" s="31"/>
+      <c r="BU16" s="31"/>
+      <c r="BV16" s="31"/>
+      <c r="BW16" s="31"/>
+      <c r="BX16" s="31"/>
+      <c r="BY16" s="31"/>
+      <c r="BZ16" s="31"/>
     </row>
-    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="45"/>
-      <c r="B17" s="61" t="s">
+    <row r="17" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="35"/>
+      <c r="B17" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="53" t="s">
+      <c r="C17" s="43" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="20">
         <v>1</v>
       </c>
-      <c r="E17" s="72">
-        <f ca="1">E15</f>
+      <c r="E17" s="61">
+        <f>E15</f>
         <v>45010</v>
       </c>
-      <c r="F17" s="72">
-        <f ca="1">E15+1</f>
+      <c r="F17" s="61">
+        <f>E15+1</f>
         <v>45011</v>
       </c>
       <c r="G17" s="14"/>
@@ -3534,25 +3682,39 @@
       <c r="BJ17" s="31"/>
       <c r="BK17" s="31"/>
       <c r="BL17" s="31"/>
+      <c r="BM17" s="31"/>
+      <c r="BN17" s="31"/>
+      <c r="BO17" s="31"/>
+      <c r="BP17" s="31"/>
+      <c r="BQ17" s="31"/>
+      <c r="BR17" s="31"/>
+      <c r="BS17" s="31"/>
+      <c r="BT17" s="31"/>
+      <c r="BU17" s="31"/>
+      <c r="BV17" s="31"/>
+      <c r="BW17" s="31"/>
+      <c r="BX17" s="31"/>
+      <c r="BY17" s="31"/>
+      <c r="BZ17" s="31"/>
     </row>
-    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="45"/>
-      <c r="B18" s="61" t="s">
+    <row r="18" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="35"/>
+      <c r="B18" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="53" t="s">
+      <c r="C18" s="43" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="20">
-        <v>0.2</v>
-      </c>
-      <c r="E18" s="72">
-        <f ca="1">F17</f>
+        <v>1</v>
+      </c>
+      <c r="E18" s="61">
+        <f>F17</f>
         <v>45011</v>
       </c>
-      <c r="F18" s="72">
-        <f ca="1">E18+5</f>
-        <v>45016</v>
+      <c r="F18" s="61">
+        <f>E18+9</f>
+        <v>45020</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
@@ -3612,21 +3774,35 @@
       <c r="BJ18" s="31"/>
       <c r="BK18" s="31"/>
       <c r="BL18" s="31"/>
+      <c r="BM18" s="31"/>
+      <c r="BN18" s="31"/>
+      <c r="BO18" s="31"/>
+      <c r="BP18" s="31"/>
+      <c r="BQ18" s="31"/>
+      <c r="BR18" s="31"/>
+      <c r="BS18" s="31"/>
+      <c r="BT18" s="31"/>
+      <c r="BU18" s="31"/>
+      <c r="BV18" s="31"/>
+      <c r="BW18" s="31"/>
+      <c r="BX18" s="31"/>
+      <c r="BY18" s="31"/>
+      <c r="BZ18" s="31"/>
     </row>
-    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="46" t="s">
+    <row r="19" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="36" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="54"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="19"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="74"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="63"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="I19" s="31"/>
@@ -3685,30 +3861,44 @@
       <c r="BJ19" s="31"/>
       <c r="BK19" s="31"/>
       <c r="BL19" s="31"/>
+      <c r="BM19" s="31"/>
+      <c r="BN19" s="31"/>
+      <c r="BO19" s="31"/>
+      <c r="BP19" s="31"/>
+      <c r="BQ19" s="31"/>
+      <c r="BR19" s="31"/>
+      <c r="BS19" s="31"/>
+      <c r="BT19" s="31"/>
+      <c r="BU19" s="31"/>
+      <c r="BV19" s="31"/>
+      <c r="BW19" s="31"/>
+      <c r="BX19" s="31"/>
+      <c r="BY19" s="31"/>
+      <c r="BZ19" s="31"/>
     </row>
-    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A20" s="46"/>
-      <c r="B20" s="62" t="s">
+    <row r="20" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="36"/>
+      <c r="B20" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="55" t="s">
+      <c r="C20" s="45" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="20">
-        <v>0</v>
-      </c>
-      <c r="E20" s="75">
-        <f ca="1">E3+9</f>
-        <v>45015</v>
-      </c>
-      <c r="F20" s="75">
-        <f ca="1">E20+1</f>
+        <v>1</v>
+      </c>
+      <c r="E20" s="64">
+        <f>F17+3</f>
+        <v>45014</v>
+      </c>
+      <c r="F20" s="64">
+        <f>E20+2</f>
         <v>45016</v>
       </c>
       <c r="G20" s="14"/>
       <c r="H20" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="17"/>
+        <v>3</v>
       </c>
       <c r="I20" s="31"/>
       <c r="J20" s="31"/>
@@ -3766,30 +3956,44 @@
       <c r="BJ20" s="31"/>
       <c r="BK20" s="31"/>
       <c r="BL20" s="31"/>
+      <c r="BM20" s="31"/>
+      <c r="BN20" s="31"/>
+      <c r="BO20" s="31"/>
+      <c r="BP20" s="31"/>
+      <c r="BQ20" s="31"/>
+      <c r="BR20" s="31"/>
+      <c r="BS20" s="31"/>
+      <c r="BT20" s="31"/>
+      <c r="BU20" s="31"/>
+      <c r="BV20" s="31"/>
+      <c r="BW20" s="31"/>
+      <c r="BX20" s="31"/>
+      <c r="BY20" s="31"/>
+      <c r="BZ20" s="31"/>
     </row>
-    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A21" s="45"/>
-      <c r="B21" s="62" t="s">
+    <row r="21" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A21" s="35"/>
+      <c r="B21" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="55" t="s">
+      <c r="C21" s="45" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="20">
-        <v>0</v>
-      </c>
-      <c r="E21" s="75">
-        <f ca="1">E20</f>
-        <v>45015</v>
-      </c>
-      <c r="F21" s="75">
-        <f ca="1">E21+1</f>
+        <v>1</v>
+      </c>
+      <c r="E21" s="64">
+        <f>E20</f>
+        <v>45014</v>
+      </c>
+      <c r="F21" s="64">
+        <f>E21+2</f>
         <v>45016</v>
       </c>
       <c r="G21" s="14"/>
       <c r="H21" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="17"/>
+        <v>3</v>
       </c>
       <c r="I21" s="31"/>
       <c r="J21" s="31"/>
@@ -3847,30 +4051,44 @@
       <c r="BJ21" s="31"/>
       <c r="BK21" s="31"/>
       <c r="BL21" s="31"/>
+      <c r="BM21" s="31"/>
+      <c r="BN21" s="31"/>
+      <c r="BO21" s="31"/>
+      <c r="BP21" s="31"/>
+      <c r="BQ21" s="31"/>
+      <c r="BR21" s="31"/>
+      <c r="BS21" s="31"/>
+      <c r="BT21" s="31"/>
+      <c r="BU21" s="31"/>
+      <c r="BV21" s="31"/>
+      <c r="BW21" s="31"/>
+      <c r="BX21" s="31"/>
+      <c r="BY21" s="31"/>
+      <c r="BZ21" s="31"/>
     </row>
-    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A22" s="45"/>
-      <c r="B22" s="62" t="s">
+    <row r="22" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A22" s="35"/>
+      <c r="B22" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="55" t="s">
+      <c r="C22" s="45" t="s">
         <v>29</v>
       </c>
       <c r="D22" s="20">
-        <v>0</v>
-      </c>
-      <c r="E22" s="75">
-        <f ca="1">E20</f>
-        <v>45015</v>
-      </c>
-      <c r="F22" s="75">
-        <f ca="1">E22+1</f>
-        <v>45016</v>
+        <v>1</v>
+      </c>
+      <c r="E22" s="64">
+        <f>E20</f>
+        <v>45014</v>
+      </c>
+      <c r="F22" s="64">
+        <f>E22+5</f>
+        <v>45019</v>
       </c>
       <c r="G22" s="14"/>
       <c r="H22" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="17"/>
+        <v>6</v>
       </c>
       <c r="I22" s="31"/>
       <c r="J22" s="31"/>
@@ -3928,22 +4146,44 @@
       <c r="BJ22" s="31"/>
       <c r="BK22" s="31"/>
       <c r="BL22" s="31"/>
+      <c r="BM22" s="31"/>
+      <c r="BN22" s="31"/>
+      <c r="BO22" s="31"/>
+      <c r="BP22" s="31"/>
+      <c r="BQ22" s="31"/>
+      <c r="BR22" s="31"/>
+      <c r="BS22" s="31"/>
+      <c r="BT22" s="31"/>
+      <c r="BU22" s="31"/>
+      <c r="BV22" s="31"/>
+      <c r="BW22" s="31"/>
+      <c r="BX22" s="31"/>
+      <c r="BY22" s="31"/>
+      <c r="BZ22" s="31"/>
     </row>
-    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A23" s="45" t="s">
+    <row r="23" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A23" s="35"/>
+      <c r="B23" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="77"/>
+      <c r="C23" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="20">
+        <v>1</v>
+      </c>
+      <c r="E23" s="64">
+        <f>E25</f>
+        <v>45017</v>
+      </c>
+      <c r="F23" s="64">
+        <f>E23+2</f>
+        <v>45019</v>
+      </c>
       <c r="G23" s="14"/>
-      <c r="H23" s="14" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
+      <c r="H23" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>3</v>
       </c>
       <c r="I23" s="31"/>
       <c r="J23" s="31"/>
@@ -4001,28 +4241,36 @@
       <c r="BJ23" s="31"/>
       <c r="BK23" s="31"/>
       <c r="BL23" s="31"/>
+      <c r="BM23" s="31"/>
+      <c r="BN23" s="31"/>
+      <c r="BO23" s="31"/>
+      <c r="BP23" s="31"/>
+      <c r="BQ23" s="31"/>
+      <c r="BR23" s="31"/>
+      <c r="BS23" s="31"/>
+      <c r="BT23" s="31"/>
+      <c r="BU23" s="31"/>
+      <c r="BV23" s="31"/>
+      <c r="BW23" s="31"/>
+      <c r="BX23" s="31"/>
+      <c r="BY23" s="31"/>
+      <c r="BZ23" s="31"/>
     </row>
-    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A24" s="45"/>
-      <c r="B24" s="63" t="s">
+    <row r="24" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A24" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="78">
-        <f ca="1">E22+1</f>
-        <v>45016</v>
-      </c>
-      <c r="F24" s="78">
-        <f ca="1">E24+3</f>
-        <v>45019</v>
-      </c>
+      <c r="C24" s="46"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="66"/>
       <c r="G24" s="14"/>
-      <c r="H24" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+      <c r="H24" s="14" t="str">
+        <f t="shared" ca="1" si="17"/>
+        <v/>
       </c>
       <c r="I24" s="31"/>
       <c r="J24" s="31"/>
@@ -4080,28 +4328,44 @@
       <c r="BJ24" s="31"/>
       <c r="BK24" s="31"/>
       <c r="BL24" s="31"/>
+      <c r="BM24" s="31"/>
+      <c r="BN24" s="31"/>
+      <c r="BO24" s="31"/>
+      <c r="BP24" s="31"/>
+      <c r="BQ24" s="31"/>
+      <c r="BR24" s="31"/>
+      <c r="BS24" s="31"/>
+      <c r="BT24" s="31"/>
+      <c r="BU24" s="31"/>
+      <c r="BV24" s="31"/>
+      <c r="BW24" s="31"/>
+      <c r="BX24" s="31"/>
+      <c r="BY24" s="31"/>
+      <c r="BZ24" s="31"/>
     </row>
-    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A25" s="45"/>
-      <c r="B25" s="63" t="s">
+    <row r="25" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A25" s="35"/>
+      <c r="B25" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="23"/>
-      <c r="E25" s="78">
-        <f ca="1">E24</f>
-        <v>45016</v>
-      </c>
-      <c r="F25" s="78">
-        <f ca="1">E24+3</f>
-        <v>45019</v>
+      <c r="C25" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="23">
+        <v>1</v>
+      </c>
+      <c r="E25" s="67">
+        <f>F21+1</f>
+        <v>45017</v>
+      </c>
+      <c r="F25" s="67">
+        <f>E25+4</f>
+        <v>45021</v>
       </c>
       <c r="G25" s="14"/>
       <c r="H25" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="17"/>
+        <v>5</v>
       </c>
       <c r="I25" s="31"/>
       <c r="J25" s="31"/>
@@ -4159,28 +4423,44 @@
       <c r="BJ25" s="31"/>
       <c r="BK25" s="31"/>
       <c r="BL25" s="31"/>
+      <c r="BM25" s="31"/>
+      <c r="BN25" s="31"/>
+      <c r="BO25" s="31"/>
+      <c r="BP25" s="31"/>
+      <c r="BQ25" s="31"/>
+      <c r="BR25" s="31"/>
+      <c r="BS25" s="31"/>
+      <c r="BT25" s="31"/>
+      <c r="BU25" s="31"/>
+      <c r="BV25" s="31"/>
+      <c r="BW25" s="31"/>
+      <c r="BX25" s="31"/>
+      <c r="BY25" s="31"/>
+      <c r="BZ25" s="31"/>
     </row>
-    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A26" s="45"/>
-      <c r="B26" s="63" t="s">
+    <row r="26" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A26" s="35"/>
+      <c r="B26" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="78">
-        <f ca="1">E24</f>
-        <v>45016</v>
-      </c>
-      <c r="F26" s="78">
-        <f ca="1">E24+3</f>
-        <v>45019</v>
+      <c r="C26" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="23">
+        <v>0</v>
+      </c>
+      <c r="E26" s="67">
+        <f>E25</f>
+        <v>45017</v>
+      </c>
+      <c r="F26" s="67">
+        <f>E25+4</f>
+        <v>45021</v>
       </c>
       <c r="G26" s="14"/>
       <c r="H26" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="17"/>
+        <v>5</v>
       </c>
       <c r="I26" s="31"/>
       <c r="J26" s="31"/>
@@ -4238,28 +4518,44 @@
       <c r="BJ26" s="31"/>
       <c r="BK26" s="31"/>
       <c r="BL26" s="31"/>
+      <c r="BM26" s="31"/>
+      <c r="BN26" s="31"/>
+      <c r="BO26" s="31"/>
+      <c r="BP26" s="31"/>
+      <c r="BQ26" s="31"/>
+      <c r="BR26" s="31"/>
+      <c r="BS26" s="31"/>
+      <c r="BT26" s="31"/>
+      <c r="BU26" s="31"/>
+      <c r="BV26" s="31"/>
+      <c r="BW26" s="31"/>
+      <c r="BX26" s="31"/>
+      <c r="BY26" s="31"/>
+      <c r="BZ26" s="31"/>
     </row>
-    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A27" s="45"/>
-      <c r="B27" s="63" t="s">
+    <row r="27" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A27" s="35"/>
+      <c r="B27" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="78">
-        <f ca="1">E24+3</f>
-        <v>45019</v>
-      </c>
-      <c r="F27" s="78">
-        <f ca="1">E24+3</f>
-        <v>45019</v>
+      <c r="C27" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="23">
+        <v>0</v>
+      </c>
+      <c r="E27" s="67">
+        <f>E25</f>
+        <v>45017</v>
+      </c>
+      <c r="F27" s="67">
+        <f>E25+4</f>
+        <v>45021</v>
       </c>
       <c r="G27" s="14"/>
       <c r="H27" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="17"/>
+        <v>5</v>
       </c>
       <c r="I27" s="31"/>
       <c r="J27" s="31"/>
@@ -4317,22 +4613,44 @@
       <c r="BJ27" s="31"/>
       <c r="BK27" s="31"/>
       <c r="BL27" s="31"/>
+      <c r="BM27" s="31"/>
+      <c r="BN27" s="31"/>
+      <c r="BO27" s="31"/>
+      <c r="BP27" s="31"/>
+      <c r="BQ27" s="31"/>
+      <c r="BR27" s="31"/>
+      <c r="BS27" s="31"/>
+      <c r="BT27" s="31"/>
+      <c r="BU27" s="31"/>
+      <c r="BV27" s="31"/>
+      <c r="BW27" s="31"/>
+      <c r="BX27" s="31"/>
+      <c r="BY27" s="31"/>
+      <c r="BZ27" s="31"/>
     </row>
-    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A28" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="21" t="s">
+    <row r="28" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A28" s="35"/>
+      <c r="B28" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="56"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="77"/>
+      <c r="C28" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="23">
+        <v>0</v>
+      </c>
+      <c r="E28" s="67">
+        <f>E25+4</f>
+        <v>45021</v>
+      </c>
+      <c r="F28" s="67">
+        <f>E25+4</f>
+        <v>45021</v>
+      </c>
       <c r="G28" s="14"/>
-      <c r="H28" s="14" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
+      <c r="H28" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>1</v>
       </c>
       <c r="I28" s="31"/>
       <c r="J28" s="31"/>
@@ -4390,28 +4708,36 @@
       <c r="BJ28" s="31"/>
       <c r="BK28" s="31"/>
       <c r="BL28" s="31"/>
+      <c r="BM28" s="31"/>
+      <c r="BN28" s="31"/>
+      <c r="BO28" s="31"/>
+      <c r="BP28" s="31"/>
+      <c r="BQ28" s="31"/>
+      <c r="BR28" s="31"/>
+      <c r="BS28" s="31"/>
+      <c r="BT28" s="31"/>
+      <c r="BU28" s="31"/>
+      <c r="BV28" s="31"/>
+      <c r="BW28" s="31"/>
+      <c r="BX28" s="31"/>
+      <c r="BY28" s="31"/>
+      <c r="BZ28" s="31"/>
     </row>
-    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A29" s="45"/>
-      <c r="B29" s="63" t="s">
+    <row r="29" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A29" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="57" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="78">
-        <f ca="1">F27+15</f>
-        <v>45034</v>
-      </c>
-      <c r="F29" s="78">
-        <f ca="1">E29</f>
-        <v>45034</v>
-      </c>
+      <c r="C29" s="46"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="66"/>
       <c r="G29" s="14"/>
-      <c r="H29" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+      <c r="H29" s="14" t="str">
+        <f t="shared" ca="1" si="17"/>
+        <v/>
       </c>
       <c r="I29" s="31"/>
       <c r="J29" s="31"/>
@@ -4469,27 +4795,41 @@
       <c r="BJ29" s="31"/>
       <c r="BK29" s="31"/>
       <c r="BL29" s="31"/>
+      <c r="BM29" s="31"/>
+      <c r="BN29" s="31"/>
+      <c r="BO29" s="31"/>
+      <c r="BP29" s="31"/>
+      <c r="BQ29" s="31"/>
+      <c r="BR29" s="31"/>
+      <c r="BS29" s="31"/>
+      <c r="BT29" s="31"/>
+      <c r="BU29" s="31"/>
+      <c r="BV29" s="31"/>
+      <c r="BW29" s="31"/>
+      <c r="BX29" s="31"/>
+      <c r="BY29" s="31"/>
+      <c r="BZ29" s="31"/>
     </row>
-    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A30" s="45"/>
-      <c r="B30" s="63" t="s">
+    <row r="30" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A30" s="35"/>
+      <c r="B30" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="57" t="s">
-        <v>27</v>
+      <c r="C30" s="47" t="s">
+        <v>24</v>
       </c>
       <c r="D30" s="23"/>
-      <c r="E30" s="78">
-        <f ca="1">E24+15</f>
-        <v>45031</v>
-      </c>
-      <c r="F30" s="78">
-        <f ca="1">E30</f>
-        <v>45031</v>
+      <c r="E30" s="67">
+        <f>F28+15</f>
+        <v>45036</v>
+      </c>
+      <c r="F30" s="67">
+        <f>E30</f>
+        <v>45036</v>
       </c>
       <c r="G30" s="14"/>
       <c r="H30" s="14">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="17"/>
         <v>1</v>
       </c>
       <c r="I30" s="31"/>
@@ -4548,22 +4888,42 @@
       <c r="BJ30" s="31"/>
       <c r="BK30" s="31"/>
       <c r="BL30" s="31"/>
+      <c r="BM30" s="31"/>
+      <c r="BN30" s="31"/>
+      <c r="BO30" s="31"/>
+      <c r="BP30" s="31"/>
+      <c r="BQ30" s="31"/>
+      <c r="BR30" s="31"/>
+      <c r="BS30" s="31"/>
+      <c r="BT30" s="31"/>
+      <c r="BU30" s="31"/>
+      <c r="BV30" s="31"/>
+      <c r="BW30" s="31"/>
+      <c r="BX30" s="31"/>
+      <c r="BY30" s="31"/>
+      <c r="BZ30" s="31"/>
     </row>
-    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A31" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="24" t="s">
+    <row r="31" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A31" s="35"/>
+      <c r="B31" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="58"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="80"/>
+      <c r="C31" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="23"/>
+      <c r="E31" s="67">
+        <f>E30</f>
+        <v>45036</v>
+      </c>
+      <c r="F31" s="67">
+        <f>E31</f>
+        <v>45036</v>
+      </c>
       <c r="G31" s="14"/>
-      <c r="H31" s="14" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
+      <c r="H31" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>1</v>
       </c>
       <c r="I31" s="31"/>
       <c r="J31" s="31"/>
@@ -4621,19 +4981,35 @@
       <c r="BJ31" s="31"/>
       <c r="BK31" s="31"/>
       <c r="BL31" s="31"/>
+      <c r="BM31" s="31"/>
+      <c r="BN31" s="31"/>
+      <c r="BO31" s="31"/>
+      <c r="BP31" s="31"/>
+      <c r="BQ31" s="31"/>
+      <c r="BR31" s="31"/>
+      <c r="BS31" s="31"/>
+      <c r="BT31" s="31"/>
+      <c r="BU31" s="31"/>
+      <c r="BV31" s="31"/>
+      <c r="BW31" s="31"/>
+      <c r="BX31" s="31"/>
+      <c r="BY31" s="31"/>
+      <c r="BZ31" s="31"/>
     </row>
-    <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A32" s="45"/>
-      <c r="B32" s="64" t="s">
+    <row r="32" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A32" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="59"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="81"/>
-      <c r="F32" s="81"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="68"/>
+      <c r="F32" s="69"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="I32" s="31"/>
@@ -4692,24 +5068,34 @@
       <c r="BJ32" s="31"/>
       <c r="BK32" s="31"/>
       <c r="BL32" s="31"/>
+      <c r="BM32" s="31"/>
+      <c r="BN32" s="31"/>
+      <c r="BO32" s="31"/>
+      <c r="BP32" s="31"/>
+      <c r="BQ32" s="31"/>
+      <c r="BR32" s="31"/>
+      <c r="BS32" s="31"/>
+      <c r="BT32" s="31"/>
+      <c r="BU32" s="31"/>
+      <c r="BV32" s="31"/>
+      <c r="BW32" s="31"/>
+      <c r="BX32" s="31"/>
+      <c r="BY32" s="31"/>
+      <c r="BZ32" s="31"/>
     </row>
-    <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A33" s="45"/>
-      <c r="B33" s="64" t="s">
+    <row r="33" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A33" s="35"/>
+      <c r="B33" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="59"/>
+      <c r="C33" s="49"/>
       <c r="D33" s="26"/>
-      <c r="E33" s="81" t="s">
-        <v>52</v>
-      </c>
-      <c r="F33" s="81" t="s">
-        <v>52</v>
-      </c>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
       <c r="G33" s="14"/>
-      <c r="H33" s="14" t="e">
-        <f t="shared" ca="1" si="6"/>
-        <v>#VALUE!</v>
+      <c r="H33" s="14" t="str">
+        <f t="shared" ca="1" si="17"/>
+        <v/>
       </c>
       <c r="I33" s="31"/>
       <c r="J33" s="31"/>
@@ -4767,23 +5153,37 @@
       <c r="BJ33" s="31"/>
       <c r="BK33" s="31"/>
       <c r="BL33" s="31"/>
+      <c r="BM33" s="31"/>
+      <c r="BN33" s="31"/>
+      <c r="BO33" s="31"/>
+      <c r="BP33" s="31"/>
+      <c r="BQ33" s="31"/>
+      <c r="BR33" s="31"/>
+      <c r="BS33" s="31"/>
+      <c r="BT33" s="31"/>
+      <c r="BU33" s="31"/>
+      <c r="BV33" s="31"/>
+      <c r="BW33" s="31"/>
+      <c r="BX33" s="31"/>
+      <c r="BY33" s="31"/>
+      <c r="BZ33" s="31"/>
     </row>
-    <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A34" s="45"/>
-      <c r="B34" s="64" t="s">
+    <row r="34" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A34" s="35"/>
+      <c r="B34" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="49"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="59"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="81" t="s">
-        <v>52</v>
-      </c>
-      <c r="F34" s="81" t="s">
-        <v>52</v>
+      <c r="F34" s="70" t="s">
+        <v>53</v>
       </c>
       <c r="G34" s="14"/>
       <c r="H34" s="14" t="e">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="17"/>
         <v>#VALUE!</v>
       </c>
       <c r="I34" s="31"/>
@@ -4842,23 +5242,37 @@
       <c r="BJ34" s="31"/>
       <c r="BK34" s="31"/>
       <c r="BL34" s="31"/>
+      <c r="BM34" s="31"/>
+      <c r="BN34" s="31"/>
+      <c r="BO34" s="31"/>
+      <c r="BP34" s="31"/>
+      <c r="BQ34" s="31"/>
+      <c r="BR34" s="31"/>
+      <c r="BS34" s="31"/>
+      <c r="BT34" s="31"/>
+      <c r="BU34" s="31"/>
+      <c r="BV34" s="31"/>
+      <c r="BW34" s="31"/>
+      <c r="BX34" s="31"/>
+      <c r="BY34" s="31"/>
+      <c r="BZ34" s="31"/>
     </row>
-    <row r="35" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A35" s="45"/>
-      <c r="B35" s="64" t="s">
+    <row r="35" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A35" s="35"/>
+      <c r="B35" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="59"/>
+      <c r="C35" s="49"/>
       <c r="D35" s="26"/>
-      <c r="E35" s="81" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" s="81" t="s">
-        <v>52</v>
+      <c r="E35" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" s="70" t="s">
+        <v>53</v>
       </c>
       <c r="G35" s="14"/>
       <c r="H35" s="14" t="e">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="17"/>
         <v>#VALUE!</v>
       </c>
       <c r="I35" s="31"/>
@@ -4917,23 +5331,37 @@
       <c r="BJ35" s="31"/>
       <c r="BK35" s="31"/>
       <c r="BL35" s="31"/>
+      <c r="BM35" s="31"/>
+      <c r="BN35" s="31"/>
+      <c r="BO35" s="31"/>
+      <c r="BP35" s="31"/>
+      <c r="BQ35" s="31"/>
+      <c r="BR35" s="31"/>
+      <c r="BS35" s="31"/>
+      <c r="BT35" s="31"/>
+      <c r="BU35" s="31"/>
+      <c r="BV35" s="31"/>
+      <c r="BW35" s="31"/>
+      <c r="BX35" s="31"/>
+      <c r="BY35" s="31"/>
+      <c r="BZ35" s="31"/>
     </row>
-    <row r="36" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A36" s="45"/>
-      <c r="B36" s="64" t="s">
+    <row r="36" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A36" s="35"/>
+      <c r="B36" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="59"/>
+      <c r="C36" s="49"/>
       <c r="D36" s="26"/>
-      <c r="E36" s="81" t="s">
-        <v>52</v>
-      </c>
-      <c r="F36" s="81" t="s">
-        <v>52</v>
+      <c r="E36" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" s="70" t="s">
+        <v>53</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14" t="e">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="17"/>
         <v>#VALUE!</v>
       </c>
       <c r="I36" s="31"/>
@@ -4992,20 +5420,38 @@
       <c r="BJ36" s="31"/>
       <c r="BK36" s="31"/>
       <c r="BL36" s="31"/>
+      <c r="BM36" s="31"/>
+      <c r="BN36" s="31"/>
+      <c r="BO36" s="31"/>
+      <c r="BP36" s="31"/>
+      <c r="BQ36" s="31"/>
+      <c r="BR36" s="31"/>
+      <c r="BS36" s="31"/>
+      <c r="BT36" s="31"/>
+      <c r="BU36" s="31"/>
+      <c r="BV36" s="31"/>
+      <c r="BW36" s="31"/>
+      <c r="BX36" s="31"/>
+      <c r="BY36" s="31"/>
+      <c r="BZ36" s="31"/>
     </row>
-    <row r="37" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A37" s="45" t="s">
+    <row r="37" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A37" s="35"/>
+      <c r="B37" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="65"/>
-      <c r="C37" s="60"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="82"/>
-      <c r="F37" s="82"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="F37" s="70" t="s">
+        <v>53</v>
+      </c>
       <c r="G37" s="14"/>
-      <c r="H37" s="14" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
+      <c r="H37" s="14" t="e">
+        <f t="shared" ca="1" si="17"/>
+        <v>#VALUE!</v>
       </c>
       <c r="I37" s="31"/>
       <c r="J37" s="31"/>
@@ -5063,106 +5509,221 @@
       <c r="BJ37" s="31"/>
       <c r="BK37" s="31"/>
       <c r="BL37" s="31"/>
+      <c r="BM37" s="31"/>
+      <c r="BN37" s="31"/>
+      <c r="BO37" s="31"/>
+      <c r="BP37" s="31"/>
+      <c r="BQ37" s="31"/>
+      <c r="BR37" s="31"/>
+      <c r="BS37" s="31"/>
+      <c r="BT37" s="31"/>
+      <c r="BU37" s="31"/>
+      <c r="BV37" s="31"/>
+      <c r="BW37" s="31"/>
+      <c r="BX37" s="31"/>
+      <c r="BY37" s="31"/>
+      <c r="BZ37" s="31"/>
     </row>
-    <row r="38" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="A38" s="46" t="s">
+    <row r="38" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A38" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="27" t="s">
+      <c r="B38" s="55"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="71"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14" t="str">
+        <f t="shared" ca="1" si="17"/>
+        <v/>
+      </c>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
+      <c r="M38" s="31"/>
+      <c r="N38" s="31"/>
+      <c r="O38" s="31"/>
+      <c r="P38" s="31"/>
+      <c r="Q38" s="31"/>
+      <c r="R38" s="31"/>
+      <c r="S38" s="31"/>
+      <c r="T38" s="31"/>
+      <c r="U38" s="31"/>
+      <c r="V38" s="31"/>
+      <c r="W38" s="31"/>
+      <c r="X38" s="31"/>
+      <c r="Y38" s="31"/>
+      <c r="Z38" s="31"/>
+      <c r="AA38" s="31"/>
+      <c r="AB38" s="31"/>
+      <c r="AC38" s="31"/>
+      <c r="AD38" s="31"/>
+      <c r="AE38" s="31"/>
+      <c r="AF38" s="31"/>
+      <c r="AG38" s="31"/>
+      <c r="AH38" s="31"/>
+      <c r="AI38" s="31"/>
+      <c r="AJ38" s="31"/>
+      <c r="AK38" s="31"/>
+      <c r="AL38" s="31"/>
+      <c r="AM38" s="31"/>
+      <c r="AN38" s="31"/>
+      <c r="AO38" s="31"/>
+      <c r="AP38" s="31"/>
+      <c r="AQ38" s="31"/>
+      <c r="AR38" s="31"/>
+      <c r="AS38" s="31"/>
+      <c r="AT38" s="31"/>
+      <c r="AU38" s="31"/>
+      <c r="AV38" s="31"/>
+      <c r="AW38" s="31"/>
+      <c r="AX38" s="31"/>
+      <c r="AY38" s="31"/>
+      <c r="AZ38" s="31"/>
+      <c r="BA38" s="31"/>
+      <c r="BB38" s="31"/>
+      <c r="BC38" s="31"/>
+      <c r="BD38" s="31"/>
+      <c r="BE38" s="31"/>
+      <c r="BF38" s="31"/>
+      <c r="BG38" s="31"/>
+      <c r="BH38" s="31"/>
+      <c r="BI38" s="31"/>
+      <c r="BJ38" s="31"/>
+      <c r="BK38" s="31"/>
+      <c r="BL38" s="31"/>
+      <c r="BM38" s="31"/>
+      <c r="BN38" s="31"/>
+      <c r="BO38" s="31"/>
+      <c r="BP38" s="31"/>
+      <c r="BQ38" s="31"/>
+      <c r="BR38" s="31"/>
+      <c r="BS38" s="31"/>
+      <c r="BT38" s="31"/>
+      <c r="BU38" s="31"/>
+      <c r="BV38" s="31"/>
+      <c r="BW38" s="31"/>
+      <c r="BX38" s="31"/>
+      <c r="BY38" s="31"/>
+      <c r="BZ38" s="31"/>
+    </row>
+    <row r="39" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A39" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="28"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="83"/>
-      <c r="F38" s="84"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30" t="str">
-        <f t="shared" ca="1" si="6"/>
+      <c r="B39" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="28"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="72"/>
+      <c r="F39" s="73"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30" t="str">
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
-      <c r="I38" s="33"/>
-      <c r="J38" s="33"/>
-      <c r="K38" s="33"/>
-      <c r="L38" s="33"/>
-      <c r="M38" s="33"/>
-      <c r="N38" s="33"/>
-      <c r="O38" s="33"/>
-      <c r="P38" s="33"/>
-      <c r="Q38" s="33"/>
-      <c r="R38" s="33"/>
-      <c r="S38" s="33"/>
-      <c r="T38" s="33"/>
-      <c r="U38" s="33"/>
-      <c r="V38" s="33"/>
-      <c r="W38" s="33"/>
-      <c r="X38" s="33"/>
-      <c r="Y38" s="33"/>
-      <c r="Z38" s="33"/>
-      <c r="AA38" s="33"/>
-      <c r="AB38" s="33"/>
-      <c r="AC38" s="33"/>
-      <c r="AD38" s="33"/>
-      <c r="AE38" s="33"/>
-      <c r="AF38" s="33"/>
-      <c r="AG38" s="33"/>
-      <c r="AH38" s="33"/>
-      <c r="AI38" s="33"/>
-      <c r="AJ38" s="33"/>
-      <c r="AK38" s="33"/>
-      <c r="AL38" s="33"/>
-      <c r="AM38" s="33"/>
-      <c r="AN38" s="33"/>
-      <c r="AO38" s="33"/>
-      <c r="AP38" s="33"/>
-      <c r="AQ38" s="33"/>
-      <c r="AR38" s="33"/>
-      <c r="AS38" s="33"/>
-      <c r="AT38" s="33"/>
-      <c r="AU38" s="33"/>
-      <c r="AV38" s="33"/>
-      <c r="AW38" s="33"/>
-      <c r="AX38" s="33"/>
-      <c r="AY38" s="33"/>
-      <c r="AZ38" s="33"/>
-      <c r="BA38" s="33"/>
-      <c r="BB38" s="33"/>
-      <c r="BC38" s="33"/>
-      <c r="BD38" s="33"/>
-      <c r="BE38" s="33"/>
-      <c r="BF38" s="33"/>
-      <c r="BG38" s="33"/>
-      <c r="BH38" s="33"/>
-      <c r="BI38" s="33"/>
-      <c r="BJ38" s="33"/>
-      <c r="BK38" s="33"/>
-      <c r="BL38" s="33"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="33"/>
+      <c r="M39" s="33"/>
+      <c r="N39" s="33"/>
+      <c r="O39" s="33"/>
+      <c r="P39" s="33"/>
+      <c r="Q39" s="33"/>
+      <c r="R39" s="33"/>
+      <c r="S39" s="33"/>
+      <c r="T39" s="33"/>
+      <c r="U39" s="33"/>
+      <c r="V39" s="33"/>
+      <c r="W39" s="33"/>
+      <c r="X39" s="33"/>
+      <c r="Y39" s="33"/>
+      <c r="Z39" s="33"/>
+      <c r="AA39" s="33"/>
+      <c r="AB39" s="33"/>
+      <c r="AC39" s="33"/>
+      <c r="AD39" s="33"/>
+      <c r="AE39" s="33"/>
+      <c r="AF39" s="33"/>
+      <c r="AG39" s="33"/>
+      <c r="AH39" s="33"/>
+      <c r="AI39" s="33"/>
+      <c r="AJ39" s="33"/>
+      <c r="AK39" s="33"/>
+      <c r="AL39" s="33"/>
+      <c r="AM39" s="33"/>
+      <c r="AN39" s="33"/>
+      <c r="AO39" s="33"/>
+      <c r="AP39" s="33"/>
+      <c r="AQ39" s="33"/>
+      <c r="AR39" s="33"/>
+      <c r="AS39" s="33"/>
+      <c r="AT39" s="33"/>
+      <c r="AU39" s="33"/>
+      <c r="AV39" s="33"/>
+      <c r="AW39" s="33"/>
+      <c r="AX39" s="33"/>
+      <c r="AY39" s="33"/>
+      <c r="AZ39" s="33"/>
+      <c r="BA39" s="33"/>
+      <c r="BB39" s="33"/>
+      <c r="BC39" s="33"/>
+      <c r="BD39" s="33"/>
+      <c r="BE39" s="33"/>
+      <c r="BF39" s="33"/>
+      <c r="BG39" s="33"/>
+      <c r="BH39" s="33"/>
+      <c r="BI39" s="33"/>
+      <c r="BJ39" s="33"/>
+      <c r="BK39" s="33"/>
+      <c r="BL39" s="33"/>
+      <c r="BM39" s="33"/>
+      <c r="BN39" s="33"/>
+      <c r="BO39" s="33"/>
+      <c r="BP39" s="33"/>
+      <c r="BQ39" s="33"/>
+      <c r="BR39" s="33"/>
+      <c r="BS39" s="33"/>
+      <c r="BT39" s="33"/>
+      <c r="BU39" s="33"/>
+      <c r="BV39" s="33"/>
+      <c r="BW39" s="33"/>
+      <c r="BX39" s="33"/>
+      <c r="BY39" s="33"/>
+      <c r="BZ39" s="33"/>
     </row>
-    <row r="39" spans="1:64" ht="30" customHeight="1">
-      <c r="G39" s="6"/>
+    <row r="40" spans="1:78" ht="30" customHeight="1">
+      <c r="G40" s="6"/>
     </row>
-    <row r="40" spans="1:64" ht="30" customHeight="1">
-      <c r="C40" s="11"/>
-      <c r="F40" s="47"/>
+    <row r="41" spans="1:78" ht="30" customHeight="1">
+      <c r="C41" s="11"/>
+      <c r="F41" s="37"/>
     </row>
-    <row r="41" spans="1:64" ht="30" customHeight="1">
-      <c r="C41" s="12"/>
+    <row r="42" spans="1:78" ht="30" customHeight="1">
+      <c r="C42" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D38">
-    <cfRule type="dataBar" priority="14">
+  <conditionalFormatting sqref="D7:D39">
+    <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5175,17 +5736,43 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL38">
-    <cfRule type="expression" dxfId="2" priority="33">
+  <conditionalFormatting sqref="I5:BL39">
+    <cfRule type="expression" dxfId="8" priority="39">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL38">
-    <cfRule type="expression" dxfId="1" priority="27">
+  <conditionalFormatting sqref="I7:BL39">
+    <cfRule type="expression" dxfId="7" priority="33">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="34" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BM5:BS39">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BM7:BS39">
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>AND(task_start&lt;=BM$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+      <formula>AND(task_end&gt;=BM$5,task_start&lt;BN$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BT5:BZ39">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>AND(TODAY()&gt;=BT$5,TODAY()&lt;BU$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BT7:BZ39">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>AND(task_start&lt;=BT$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BT$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+      <formula>AND(task_end&gt;=BT$5,task_start&lt;BU$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -5216,7 +5803,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D38</xm:sqref>
+          <xm:sqref>D7:D39</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -5224,121 +5811,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1"/>
-  <cols>
-    <col min="1" max="1" width="87.140625" style="35" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1"/>
-    <row r="2" spans="1:2" s="37" customFormat="1" ht="15.95">
-      <c r="A2" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="36"/>
-    </row>
-    <row r="3" spans="1:2" s="41" customFormat="1" ht="27" customHeight="1">
-      <c r="A3" s="69" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="42"/>
-    </row>
-    <row r="4" spans="1:2" s="38" customFormat="1" ht="26.1">
-      <c r="A4" s="39" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1">
-      <c r="A5" s="40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1">
-      <c r="A6" s="39" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="35" customFormat="1" ht="204.95" customHeight="1">
-      <c r="A7" s="44" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="38" customFormat="1" ht="26.1">
-      <c r="A8" s="39" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="48">
-      <c r="A9" s="40" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="35" customFormat="1" ht="27.95" customHeight="1">
-      <c r="A10" s="43" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" s="38" customFormat="1" ht="26.1">
-      <c r="A11" s="39" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="32.1">
-      <c r="A12" s="40" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="35" customFormat="1" ht="27.95" customHeight="1">
-      <c r="A13" s="43" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="38" customFormat="1" ht="26.1">
-      <c r="A14" s="39" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1">
-      <c r="A15" s="40" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="63.95">
-      <c r="A16" s="40" t="s">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A13" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A10" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="A2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
-  <drawing r:id="rId6"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -5356,6 +5829,15 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5647,11 +6129,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
docs: added updated work plan
</commit_message>
<xml_diff>
--- a/Gantt-Chart-Work-Plan.xlsx
+++ b/Gantt-Chart-Work-Plan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26330"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3784F6A0-4AC1-443A-9BDA-5CD7829641F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="286" documentId="8_{73792710-4ABC-C64A-8DA5-499DBBA00DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{072794E7-479B-4044-8129-545B39D0C59B}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
   <si>
     <t>Create a Project Schedule in this worksheet.
 Enter title of this project in cell B1. 
@@ -241,7 +241,10 @@
     <t>get feedback from tutor</t>
   </si>
   <si>
-    <t>zip folder + cloning summary</t>
+    <t>cloning summary</t>
+  </si>
+  <si>
+    <t>add source codes</t>
   </si>
   <si>
     <t>Stage 2 Planning</t>
@@ -1916,11 +1919,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BZ42"/>
+  <dimension ref="A1:BZ43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1"/>
@@ -2784,7 +2787,7 @@
       <c r="F8" s="60"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="str">
-        <f t="shared" ref="H8:H39" ca="1" si="17">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H40" ca="1" si="17">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="31"/>
@@ -4447,7 +4450,7 @@
         <v>34</v>
       </c>
       <c r="D26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="67">
         <f>E25</f>
@@ -4542,20 +4545,20 @@
         <v>29</v>
       </c>
       <c r="D27" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="67">
         <f>E25</f>
         <v>45017</v>
       </c>
       <c r="F27" s="67">
-        <f>E25+4</f>
-        <v>45021</v>
+        <f>E25+5</f>
+        <v>45022</v>
       </c>
       <c r="G27" s="14"/>
       <c r="H27" s="14">
         <f t="shared" ca="1" si="17"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I27" s="31"/>
       <c r="J27" s="31"/>
@@ -4637,20 +4640,20 @@
         <v>27</v>
       </c>
       <c r="D28" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="67">
         <f>E25+4</f>
         <v>45021</v>
       </c>
       <c r="F28" s="67">
-        <f>E25+4</f>
-        <v>45021</v>
+        <f>E25+5</f>
+        <v>45022</v>
       </c>
       <c r="G28" s="14"/>
       <c r="H28" s="14">
         <f t="shared" ca="1" si="17"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I28" s="31"/>
       <c r="J28" s="31"/>
@@ -4818,14 +4821,16 @@
       <c r="C30" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="23"/>
+      <c r="D30" s="23">
+        <v>0</v>
+      </c>
       <c r="E30" s="67">
-        <f>F28+15</f>
-        <v>45036</v>
+        <f>F28+12</f>
+        <v>45034</v>
       </c>
       <c r="F30" s="67">
         <f>E30</f>
-        <v>45036</v>
+        <v>45034</v>
       </c>
       <c r="G30" s="14"/>
       <c r="H30" s="14">
@@ -4911,14 +4916,16 @@
       <c r="C31" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="23"/>
+      <c r="D31" s="23">
+        <v>1</v>
+      </c>
       <c r="E31" s="67">
-        <f>E30</f>
-        <v>45036</v>
+        <f>F28+1</f>
+        <v>45023</v>
       </c>
       <c r="F31" s="67">
         <f>E31</f>
-        <v>45036</v>
+        <v>45023</v>
       </c>
       <c r="G31" s="14"/>
       <c r="H31" s="14">
@@ -4997,20 +5004,28 @@
       <c r="BZ31" s="31"/>
     </row>
     <row r="32" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A32" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="24" t="s">
+      <c r="A32" s="35"/>
+      <c r="B32" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="48"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="68"/>
-      <c r="F32" s="69"/>
+      <c r="C32" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="23">
+        <v>0</v>
+      </c>
+      <c r="E32" s="67">
+        <f>E30</f>
+        <v>45034</v>
+      </c>
+      <c r="F32" s="67">
+        <f>E32</f>
+        <v>45034</v>
+      </c>
       <c r="G32" s="14"/>
-      <c r="H32" s="14" t="str">
+      <c r="H32" s="14">
         <f t="shared" ca="1" si="17"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I32" s="31"/>
       <c r="J32" s="31"/>
@@ -5084,14 +5099,16 @@
       <c r="BZ32" s="31"/>
     </row>
     <row r="33" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A33" s="35"/>
-      <c r="B33" s="54" t="s">
+      <c r="A33" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="49"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="70"/>
-      <c r="F33" s="70"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="68"/>
+      <c r="F33" s="69"/>
       <c r="G33" s="14"/>
       <c r="H33" s="14" t="str">
         <f t="shared" ca="1" si="17"/>
@@ -5175,16 +5192,12 @@
       </c>
       <c r="C34" s="49"/>
       <c r="D34" s="26"/>
-      <c r="E34" s="70" t="s">
-        <v>53</v>
-      </c>
-      <c r="F34" s="70" t="s">
-        <v>53</v>
-      </c>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
       <c r="G34" s="14"/>
-      <c r="H34" s="14" t="e">
+      <c r="H34" s="14" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="I34" s="31"/>
       <c r="J34" s="31"/>
@@ -5260,15 +5273,15 @@
     <row r="35" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A35" s="35"/>
       <c r="B35" s="54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35" s="49"/>
       <c r="D35" s="26"/>
       <c r="E35" s="70" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F35" s="70" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G35" s="14"/>
       <c r="H35" s="14" t="e">
@@ -5354,10 +5367,10 @@
       <c r="C36" s="49"/>
       <c r="D36" s="26"/>
       <c r="E36" s="70" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F36" s="70" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14" t="e">
@@ -5443,10 +5456,10 @@
       <c r="C37" s="49"/>
       <c r="D37" s="26"/>
       <c r="E37" s="70" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F37" s="70" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G37" s="14"/>
       <c r="H37" s="14" t="e">
@@ -5525,18 +5538,22 @@
       <c r="BZ37" s="31"/>
     </row>
     <row r="38" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="35"/>
+      <c r="B38" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="55"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="71"/>
-      <c r="F38" s="71"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="F38" s="70" t="s">
+        <v>54</v>
+      </c>
       <c r="G38" s="14"/>
-      <c r="H38" s="14" t="str">
+      <c r="H38" s="14" t="e">
         <f t="shared" ca="1" si="17"/>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="I38" s="31"/>
       <c r="J38" s="31"/>
@@ -5610,101 +5627,186 @@
       <c r="BZ38" s="31"/>
     </row>
     <row r="39" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" s="28"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="72"/>
-      <c r="F39" s="73"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30" t="str">
+      <c r="B39" s="55"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="71"/>
+      <c r="F39" s="71"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14" t="str">
         <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
-      <c r="I39" s="33"/>
-      <c r="J39" s="33"/>
-      <c r="K39" s="33"/>
-      <c r="L39" s="33"/>
-      <c r="M39" s="33"/>
-      <c r="N39" s="33"/>
-      <c r="O39" s="33"/>
-      <c r="P39" s="33"/>
-      <c r="Q39" s="33"/>
-      <c r="R39" s="33"/>
-      <c r="S39" s="33"/>
-      <c r="T39" s="33"/>
-      <c r="U39" s="33"/>
-      <c r="V39" s="33"/>
-      <c r="W39" s="33"/>
-      <c r="X39" s="33"/>
-      <c r="Y39" s="33"/>
-      <c r="Z39" s="33"/>
-      <c r="AA39" s="33"/>
-      <c r="AB39" s="33"/>
-      <c r="AC39" s="33"/>
-      <c r="AD39" s="33"/>
-      <c r="AE39" s="33"/>
-      <c r="AF39" s="33"/>
-      <c r="AG39" s="33"/>
-      <c r="AH39" s="33"/>
-      <c r="AI39" s="33"/>
-      <c r="AJ39" s="33"/>
-      <c r="AK39" s="33"/>
-      <c r="AL39" s="33"/>
-      <c r="AM39" s="33"/>
-      <c r="AN39" s="33"/>
-      <c r="AO39" s="33"/>
-      <c r="AP39" s="33"/>
-      <c r="AQ39" s="33"/>
-      <c r="AR39" s="33"/>
-      <c r="AS39" s="33"/>
-      <c r="AT39" s="33"/>
-      <c r="AU39" s="33"/>
-      <c r="AV39" s="33"/>
-      <c r="AW39" s="33"/>
-      <c r="AX39" s="33"/>
-      <c r="AY39" s="33"/>
-      <c r="AZ39" s="33"/>
-      <c r="BA39" s="33"/>
-      <c r="BB39" s="33"/>
-      <c r="BC39" s="33"/>
-      <c r="BD39" s="33"/>
-      <c r="BE39" s="33"/>
-      <c r="BF39" s="33"/>
-      <c r="BG39" s="33"/>
-      <c r="BH39" s="33"/>
-      <c r="BI39" s="33"/>
-      <c r="BJ39" s="33"/>
-      <c r="BK39" s="33"/>
-      <c r="BL39" s="33"/>
-      <c r="BM39" s="33"/>
-      <c r="BN39" s="33"/>
-      <c r="BO39" s="33"/>
-      <c r="BP39" s="33"/>
-      <c r="BQ39" s="33"/>
-      <c r="BR39" s="33"/>
-      <c r="BS39" s="33"/>
-      <c r="BT39" s="33"/>
-      <c r="BU39" s="33"/>
-      <c r="BV39" s="33"/>
-      <c r="BW39" s="33"/>
-      <c r="BX39" s="33"/>
-      <c r="BY39" s="33"/>
-      <c r="BZ39" s="33"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="P39" s="31"/>
+      <c r="Q39" s="31"/>
+      <c r="R39" s="31"/>
+      <c r="S39" s="31"/>
+      <c r="T39" s="31"/>
+      <c r="U39" s="31"/>
+      <c r="V39" s="31"/>
+      <c r="W39" s="31"/>
+      <c r="X39" s="31"/>
+      <c r="Y39" s="31"/>
+      <c r="Z39" s="31"/>
+      <c r="AA39" s="31"/>
+      <c r="AB39" s="31"/>
+      <c r="AC39" s="31"/>
+      <c r="AD39" s="31"/>
+      <c r="AE39" s="31"/>
+      <c r="AF39" s="31"/>
+      <c r="AG39" s="31"/>
+      <c r="AH39" s="31"/>
+      <c r="AI39" s="31"/>
+      <c r="AJ39" s="31"/>
+      <c r="AK39" s="31"/>
+      <c r="AL39" s="31"/>
+      <c r="AM39" s="31"/>
+      <c r="AN39" s="31"/>
+      <c r="AO39" s="31"/>
+      <c r="AP39" s="31"/>
+      <c r="AQ39" s="31"/>
+      <c r="AR39" s="31"/>
+      <c r="AS39" s="31"/>
+      <c r="AT39" s="31"/>
+      <c r="AU39" s="31"/>
+      <c r="AV39" s="31"/>
+      <c r="AW39" s="31"/>
+      <c r="AX39" s="31"/>
+      <c r="AY39" s="31"/>
+      <c r="AZ39" s="31"/>
+      <c r="BA39" s="31"/>
+      <c r="BB39" s="31"/>
+      <c r="BC39" s="31"/>
+      <c r="BD39" s="31"/>
+      <c r="BE39" s="31"/>
+      <c r="BF39" s="31"/>
+      <c r="BG39" s="31"/>
+      <c r="BH39" s="31"/>
+      <c r="BI39" s="31"/>
+      <c r="BJ39" s="31"/>
+      <c r="BK39" s="31"/>
+      <c r="BL39" s="31"/>
+      <c r="BM39" s="31"/>
+      <c r="BN39" s="31"/>
+      <c r="BO39" s="31"/>
+      <c r="BP39" s="31"/>
+      <c r="BQ39" s="31"/>
+      <c r="BR39" s="31"/>
+      <c r="BS39" s="31"/>
+      <c r="BT39" s="31"/>
+      <c r="BU39" s="31"/>
+      <c r="BV39" s="31"/>
+      <c r="BW39" s="31"/>
+      <c r="BX39" s="31"/>
+      <c r="BY39" s="31"/>
+      <c r="BZ39" s="31"/>
     </row>
-    <row r="40" spans="1:78" ht="30" customHeight="1">
-      <c r="G40" s="6"/>
+    <row r="40" spans="1:78" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A40" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="28"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="72"/>
+      <c r="F40" s="73"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30" t="str">
+        <f t="shared" ca="1" si="17"/>
+        <v/>
+      </c>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="33"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="33"/>
+      <c r="O40" s="33"/>
+      <c r="P40" s="33"/>
+      <c r="Q40" s="33"/>
+      <c r="R40" s="33"/>
+      <c r="S40" s="33"/>
+      <c r="T40" s="33"/>
+      <c r="U40" s="33"/>
+      <c r="V40" s="33"/>
+      <c r="W40" s="33"/>
+      <c r="X40" s="33"/>
+      <c r="Y40" s="33"/>
+      <c r="Z40" s="33"/>
+      <c r="AA40" s="33"/>
+      <c r="AB40" s="33"/>
+      <c r="AC40" s="33"/>
+      <c r="AD40" s="33"/>
+      <c r="AE40" s="33"/>
+      <c r="AF40" s="33"/>
+      <c r="AG40" s="33"/>
+      <c r="AH40" s="33"/>
+      <c r="AI40" s="33"/>
+      <c r="AJ40" s="33"/>
+      <c r="AK40" s="33"/>
+      <c r="AL40" s="33"/>
+      <c r="AM40" s="33"/>
+      <c r="AN40" s="33"/>
+      <c r="AO40" s="33"/>
+      <c r="AP40" s="33"/>
+      <c r="AQ40" s="33"/>
+      <c r="AR40" s="33"/>
+      <c r="AS40" s="33"/>
+      <c r="AT40" s="33"/>
+      <c r="AU40" s="33"/>
+      <c r="AV40" s="33"/>
+      <c r="AW40" s="33"/>
+      <c r="AX40" s="33"/>
+      <c r="AY40" s="33"/>
+      <c r="AZ40" s="33"/>
+      <c r="BA40" s="33"/>
+      <c r="BB40" s="33"/>
+      <c r="BC40" s="33"/>
+      <c r="BD40" s="33"/>
+      <c r="BE40" s="33"/>
+      <c r="BF40" s="33"/>
+      <c r="BG40" s="33"/>
+      <c r="BH40" s="33"/>
+      <c r="BI40" s="33"/>
+      <c r="BJ40" s="33"/>
+      <c r="BK40" s="33"/>
+      <c r="BL40" s="33"/>
+      <c r="BM40" s="33"/>
+      <c r="BN40" s="33"/>
+      <c r="BO40" s="33"/>
+      <c r="BP40" s="33"/>
+      <c r="BQ40" s="33"/>
+      <c r="BR40" s="33"/>
+      <c r="BS40" s="33"/>
+      <c r="BT40" s="33"/>
+      <c r="BU40" s="33"/>
+      <c r="BV40" s="33"/>
+      <c r="BW40" s="33"/>
+      <c r="BX40" s="33"/>
+      <c r="BY40" s="33"/>
+      <c r="BZ40" s="33"/>
     </row>
     <row r="41" spans="1:78" ht="30" customHeight="1">
-      <c r="C41" s="11"/>
-      <c r="F41" s="37"/>
+      <c r="G41" s="6"/>
     </row>
     <row r="42" spans="1:78" ht="30" customHeight="1">
-      <c r="C42" s="12"/>
+      <c r="C42" s="11"/>
+      <c r="F42" s="37"/>
+    </row>
+    <row r="43" spans="1:78" ht="30" customHeight="1">
+      <c r="C43" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -5722,7 +5824,7 @@
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D39">
+  <conditionalFormatting sqref="D7:D40">
     <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5736,12 +5838,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL39">
+  <conditionalFormatting sqref="I5:BL40">
     <cfRule type="expression" dxfId="8" priority="39">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL39">
+  <conditionalFormatting sqref="I7:BL40">
     <cfRule type="expression" dxfId="7" priority="33">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -5749,12 +5851,12 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM5:BS39">
+  <conditionalFormatting sqref="BM5:BS40">
     <cfRule type="expression" dxfId="5" priority="6">
       <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM7:BS39">
+  <conditionalFormatting sqref="BM7:BS40">
     <cfRule type="expression" dxfId="4" priority="4">
       <formula>AND(task_start&lt;=BM$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$5)</formula>
     </cfRule>
@@ -5762,12 +5864,12 @@
       <formula>AND(task_end&gt;=BM$5,task_start&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BT5:BZ39">
+  <conditionalFormatting sqref="BT5:BZ40">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>AND(TODAY()&gt;=BT$5,TODAY()&lt;BU$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BT7:BZ39">
+  <conditionalFormatting sqref="BT7:BZ40">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>AND(task_start&lt;=BT$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BT$5)</formula>
     </cfRule>
@@ -5803,7 +5905,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D39</xm:sqref>
+          <xm:sqref>D7:D40</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>